<commit_message>
New simpler buck-only design
Bridge rectifier on input to allow reverse voltage
Voltage regulation is taken care of by ASIC
External microcontroller and OLED display show power/voltage/current
</commit_message>
<xml_diff>
--- a/digikey cart.xlsx
+++ b/digikey cart.xlsx
@@ -197,61 +197,67 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="10.4" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="3" max="3" width="35.1" customWidth="1"/>
     <col min="4" max="4" width="31.200000000000003" customWidth="1"/>
     <col min="5" max="5" width="41.6" customWidth="1"/>
     <col min="6" max="6" width="23.400000000000002" customWidth="1"/>
     <col min="7" max="7" width="11.700000000000001" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="18.2" customWidth="1"/>
+    <col min="8" max="8" width="11.700000000000001" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="23.400000000000002" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="inlineStr" r="A1" s="2">
         <is>
-          <t>#</t>
+          <t>Index</t>
         </is>
       </c>
       <c t="inlineStr" r="B1" s="2">
         <is>
-          <t>QUANTITY</t>
+          <t>Quantity</t>
         </is>
       </c>
       <c t="inlineStr" r="C1" s="2">
         <is>
-          <t>PART NUMBER</t>
+          <t>Part Number</t>
         </is>
       </c>
       <c t="inlineStr" r="D1" s="2">
         <is>
-          <t>MANUFACTURER PART NUMBER</t>
+          <t>Manufacturer Part Number</t>
         </is>
       </c>
       <c t="inlineStr" r="E1" s="2">
         <is>
-          <t>DESCRIPTION</t>
+          <t>Description</t>
         </is>
       </c>
       <c t="inlineStr" r="F1" s="2">
         <is>
-          <t>CUSTOMER REFERENCE</t>
+          <t>Customer Reference</t>
         </is>
       </c>
       <c t="inlineStr" r="G1" s="2">
         <is>
-          <t>BACKORDER</t>
+          <t>Available</t>
         </is>
       </c>
       <c t="inlineStr" r="H1" s="2">
         <is>
-          <t>UNIT PRICE</t>
+          <t>Backorder</t>
         </is>
       </c>
       <c t="inlineStr" r="I1" s="2">
         <is>
-          <t>EXTENDED PRICE</t>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J1" s="2">
+        <is>
+          <t>Extended Price USD</t>
         </is>
       </c>
     </row>
@@ -260,36 +266,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="65">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c t="inlineStr" r="C2">
         <is>
-          <t>IRS10752LTRPBFCT-ND</t>
+          <t>RMCF0603FT30K1CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D2">
         <is>
-          <t>IRS10752LTRPBF</t>
+          <t>RMCF0603FT30K1</t>
         </is>
       </c>
       <c t="inlineStr" r="E2">
         <is>
-          <t>IC GATE DRVR HIGH-SIDE SOT23-6</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F2">
-        <is>
-          <t>U2</t>
+          <t>RES 30.1K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G2" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H2">
-        <v>0.87000</v>
-      </c>
-      <c r="I2" s="66">
-        <v>2.61</v>
+        <v>20</v>
+      </c>
+      <c r="H2" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I2">
+        <v>0.01500</v>
+      </c>
+      <c r="J2" s="66">
+        <v>0.30</v>
       </c>
     </row>
     <row r="3">
@@ -297,36 +301,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="65">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t>596-1641-1-ND</t>
+          <t>RMCF0603FT31K6CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D3">
         <is>
-          <t>CHY100D-TL</t>
+          <t>RMCF0603FT31K6</t>
         </is>
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t>IC BATT USB CHARGER 8SO</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F3">
-        <is>
-          <t>U1</t>
+          <t>RES 31.6K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G3" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H3">
-        <v>0.45000</v>
-      </c>
-      <c r="I3" s="66">
-        <v>1.35</v>
+        <v>10</v>
+      </c>
+      <c r="H3" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I3">
+        <v>0.01500</v>
+      </c>
+      <c r="J3" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="4">
@@ -334,36 +336,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="65">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t>3757-PJD25N03_L2_00001CT-ND</t>
+          <t>RMCF0603FT42K2CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D4">
         <is>
-          <t>PJD25N03_L2_00001</t>
+          <t>RMCF0603FT42K2</t>
         </is>
       </c>
       <c t="inlineStr" r="E4">
         <is>
-          <t>30V N-CHANNEL ENHANCEMENT MODE M</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F4">
-        <is>
-          <t>Q1,Q2</t>
+          <t>RES 42.2K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G4" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H4">
-        <v>0.41000</v>
-      </c>
-      <c r="I4" s="66">
-        <v>2.46</v>
+        <v>10</v>
+      </c>
+      <c r="H4" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I4">
+        <v>0.01500</v>
+      </c>
+      <c r="J4" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="5">
@@ -371,36 +371,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="65">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C5">
         <is>
-          <t>ATTINY404-SSNRCT-ND</t>
+          <t>RMCF0603FT15K8CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D5">
         <is>
-          <t>ATTINY404-SSNR</t>
+          <t>RMCF0603FT15K8</t>
         </is>
       </c>
       <c t="inlineStr" r="E5">
         <is>
-          <t>IC MCU 8BIT 4KB FLASH 14SOIC</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F5">
-        <is>
-          <t>U3</t>
+          <t>RES 15.8K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G5" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H5">
-        <v>0.64000</v>
-      </c>
-      <c r="I5" s="66">
-        <v>1.92</v>
+        <v>10</v>
+      </c>
+      <c r="H5" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I5">
+        <v>0.01500</v>
+      </c>
+      <c r="J5" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
@@ -408,36 +406,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="65">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c t="inlineStr" r="C6">
         <is>
-          <t>31-AP7375-50SA-7CT-ND</t>
+          <t>RMCF0603FT158KCT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D6">
         <is>
-          <t>AP7375-50SA-7</t>
+          <t>RMCF0603FT158K</t>
         </is>
       </c>
       <c t="inlineStr" r="E6">
         <is>
-          <t>LDOCMOSLOWCURRSOT23T&amp;R3K</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F6">
-        <is>
-          <t>U4,U5</t>
+          <t>RES 158K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G6" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H6">
-        <v>0.41000</v>
-      </c>
-      <c r="I6" s="66">
-        <v>2.46</v>
+        <v>20</v>
+      </c>
+      <c r="H6" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I6">
+        <v>0.01500</v>
+      </c>
+      <c r="J6" s="66">
+        <v>0.30</v>
       </c>
     </row>
     <row r="7">
@@ -449,32 +445,30 @@
       </c>
       <c t="inlineStr" r="C7">
         <is>
-          <t>296-47655-1-ND</t>
+          <t>31-AP63300WU-7CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D7">
         <is>
-          <t>INA180A4IDBVR</t>
+          <t>AP63300WU-7</t>
         </is>
       </c>
       <c t="inlineStr" r="E7">
         <is>
-          <t>IC CURR SENSE 1 CIRCUIT SOT23-5</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F7">
-        <is>
-          <t>U6</t>
+          <t>IC REG BUCK ADJ 3A TSOT26</t>
         </is>
       </c>
       <c r="G7" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H7">
-        <v>0.40000</v>
-      </c>
-      <c r="I7" s="66">
-        <v>1.20</v>
+        <v>3</v>
+      </c>
+      <c r="H7" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I7">
+        <v>0.92000</v>
+      </c>
+      <c r="J7" s="66">
+        <v>2.76</v>
       </c>
     </row>
     <row r="8">
@@ -482,36 +476,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="65">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c t="inlineStr" r="C8">
         <is>
-          <t>3757-SBM54ALAFC_R1_00001CT-ND</t>
+          <t>3757-TS360ILS_R1_00001CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D8">
         <is>
-          <t>SBM54ALAFC_R1_00001</t>
+          <t>TS360ILS_R1_00001</t>
         </is>
       </c>
       <c t="inlineStr" r="E8">
         <is>
-          <t>DIODE SCHOTTKY 45V 5A SMAF-C</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F8">
-        <is>
-          <t>D2,D6</t>
+          <t>MICRO SURFACE MOUNT SCHOTTKY BRI</t>
         </is>
       </c>
       <c r="G8" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H8">
-        <v>0.27300</v>
-      </c>
-      <c r="I8" s="66">
-        <v>2.73</v>
+        <v>3</v>
+      </c>
+      <c r="H8" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I8">
+        <v>0.58000</v>
+      </c>
+      <c r="J8" s="66">
+        <v>1.74</v>
       </c>
     </row>
     <row r="9">
@@ -519,36 +511,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="65">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c t="inlineStr" r="C9">
         <is>
-          <t>4463-D1MPC1206QR020FF-T5CT-ND</t>
+          <t>4713-GMC31X7R106K50NTCT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D9">
         <is>
-          <t>D1MPC1206QR020FF-T5</t>
+          <t>GMC31X7R106K50NT</t>
         </is>
       </c>
       <c t="inlineStr" r="E9">
         <is>
-          <t>RES 0.02 OHM 1% 1W 1206</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F9">
-        <is>
-          <t>R12</t>
+          <t>CAP1206 X7R 10UF 10% 50V</t>
         </is>
       </c>
       <c r="G9" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H9">
-        <v>0.36000</v>
-      </c>
-      <c r="I9" s="66">
-        <v>1.08</v>
+        <v>15</v>
+      </c>
+      <c r="H9" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I9">
+        <v>0.21600</v>
+      </c>
+      <c r="J9" s="66">
+        <v>3.24</v>
       </c>
     </row>
     <row r="10">
@@ -560,32 +550,30 @@
       </c>
       <c t="inlineStr" r="C10">
         <is>
-          <t>3222-HSC1HM101GARE00RS103CT-ND</t>
+          <t>4816-HPC6045NC-3R3MCT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D10">
         <is>
-          <t>HSC1HM101GARE00RS103</t>
+          <t>HPC 6045NC-3R3M</t>
         </is>
       </c>
       <c t="inlineStr" r="E10">
         <is>
-          <t>CAP ALUM HYB 100UF 20% 50V SMD</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F10">
-        <is>
-          <t>C9,C10,C11</t>
+          <t>3.3 UH SHIELDED DRUM CORE, WIREW</t>
         </is>
       </c>
       <c r="G10" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H10">
-        <v>0.23600</v>
-      </c>
-      <c r="I10" s="66">
-        <v>2.36</v>
+        <v>10</v>
+      </c>
+      <c r="H10" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I10">
+        <v>0.16100</v>
+      </c>
+      <c r="J10" s="66">
+        <v>1.61</v>
       </c>
     </row>
     <row r="11">
@@ -593,36 +581,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="65">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C11">
         <is>
-          <t>1276-1009-1-ND</t>
+          <t>RMCF0603FT390KCT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D11">
         <is>
-          <t>CL10B103KB8NNNC</t>
+          <t>RMCF0603FT390K</t>
         </is>
       </c>
       <c t="inlineStr" r="E11">
         <is>
-          <t>CAP CER 10000PF 50V X7R 0603</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F11">
-        <is>
-          <t>C1-C8</t>
+          <t>RES 390K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G11" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H11">
-        <v>0.01340</v>
-      </c>
-      <c r="I11" s="66">
-        <v>0.67</v>
+        <v>10</v>
+      </c>
+      <c r="H11" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I11">
+        <v>0.01500</v>
+      </c>
+      <c r="J11" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="12">
@@ -634,32 +620,30 @@
       </c>
       <c t="inlineStr" r="C12">
         <is>
-          <t>RMCF0603FT402KCT-ND</t>
+          <t>RMCF0603FT4K53CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D12">
         <is>
-          <t>RMCF0603FT402K</t>
+          <t>RMCF0603FT4K53</t>
         </is>
       </c>
       <c t="inlineStr" r="E12">
         <is>
-          <t>RES 402K OHM 1% 1/10W 0603</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F12">
-        <is>
-          <t>R1,R8,R10</t>
+          <t>RES 4.53K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G12" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H12">
-        <v>0.01400</v>
-      </c>
-      <c r="I12" s="66">
-        <v>0.14</v>
+        <v>10</v>
+      </c>
+      <c r="H12" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I12">
+        <v>0.01500</v>
+      </c>
+      <c r="J12" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="13">
@@ -667,36 +651,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="65">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C13">
         <is>
-          <t>2987-CU01SAH0S00-ND</t>
+          <t>13-PA0805FRF870R005LCT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D13">
         <is>
-          <t>CU01SAH0S00</t>
+          <t>PA0805FRF870R005L</t>
         </is>
       </c>
       <c t="inlineStr" r="E13">
         <is>
-          <t>USB TYPE-A SINGLE PORT RIGHT ANG</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F13">
-        <is>
-          <t>J2</t>
+          <t>RES 0.005 OHM 1% 1W 0805</t>
         </is>
       </c>
       <c r="G13" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H13">
-        <v>0.48000</v>
-      </c>
-      <c r="I13" s="66">
-        <v>1.44</v>
+        <v>10</v>
+      </c>
+      <c r="H13" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I13">
+        <v>0.25400</v>
+      </c>
+      <c r="J13" s="66">
+        <v>2.54</v>
       </c>
     </row>
     <row r="14">
@@ -708,32 +690,30 @@
       </c>
       <c t="inlineStr" r="C14">
         <is>
-          <t>4530-1N4148WCT-ND</t>
+          <t>RMCF0603FT17K4CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D14">
         <is>
-          <t>1N4148W</t>
+          <t>RMCF0603FT17K4</t>
         </is>
       </c>
       <c t="inlineStr" r="E14">
         <is>
-          <t>400MW SURFACE MOUNT SWITCHING DI</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F14">
-        <is>
-          <t>D1</t>
+          <t>RES 17.4K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G14" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H14">
-        <v>0.04900</v>
-      </c>
-      <c r="I14" s="66">
-        <v>0.49</v>
+        <v>10</v>
+      </c>
+      <c r="H14" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I14">
+        <v>0.01500</v>
+      </c>
+      <c r="J14" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="15">
@@ -741,31 +721,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="65">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c t="inlineStr" r="C15">
         <is>
-          <t>535-AMDLA1306Q-470MTCT-ND</t>
+          <t>RMCF0603FT93K1CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D15">
         <is>
-          <t>AMDLA1306Q-470MT</t>
+          <t>RMCF0603FT93K1</t>
         </is>
       </c>
       <c t="inlineStr" r="E15">
         <is>
-          <t>FIXED IND 47UH 5.7A 67 MOHM SMD</t>
+          <t>RES 93.1K OHM 1% 1/10W 0603</t>
         </is>
       </c>
       <c r="G15" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H15">
-        <v>1.42000</v>
-      </c>
-      <c r="I15" s="66">
-        <v>1.42</v>
+        <v>10</v>
+      </c>
+      <c r="H15" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I15">
+        <v>0.01500</v>
+      </c>
+      <c r="J15" s="66">
+        <v>0.15</v>
       </c>
     </row>
     <row r="16">
@@ -773,31 +756,69 @@
         <v>15</v>
       </c>
       <c r="B16" s="65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c t="inlineStr" r="C16">
         <is>
-          <t>811-2463-ND</t>
+          <t>31-AP64060WU-7CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D16">
         <is>
-          <t>60B224C</t>
+          <t>AP64060WU-7</t>
         </is>
       </c>
       <c t="inlineStr" r="E16">
         <is>
-          <t>FIXED IND 220UH 5A 50 MOHM SMD</t>
+          <t>IC REG BUCK ADJ 600MA TSOT26</t>
         </is>
       </c>
       <c r="G16" s="65">
-        <v>0</v>
-      </c>
-      <c t="n" r="H16">
-        <v>2.20000</v>
-      </c>
-      <c r="I16" s="66">
-        <v>2.20</v>
+        <v>3</v>
+      </c>
+      <c r="H16" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I16">
+        <v>0.62000</v>
+      </c>
+      <c r="J16" s="66">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="65">
+        <v>16</v>
+      </c>
+      <c r="B17" s="65">
+        <v>4</v>
+      </c>
+      <c t="inlineStr" r="C17">
+        <is>
+          <t>445-6762-1-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D17">
+        <is>
+          <t>MLZ2012N100LT000</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E17">
+        <is>
+          <t>FIXED IND 10UH 500MA 300MOHM SMD</t>
+        </is>
+      </c>
+      <c r="G17" s="65">
+        <v>4</v>
+      </c>
+      <c r="H17" s="65">
+        <v>0</v>
+      </c>
+      <c t="n" r="I17">
+        <v>0.12000</v>
+      </c>
+      <c r="J17" s="66">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>